<commit_message>
last edits Inshaa allah
</commit_message>
<xml_diff>
--- a/Attendance_Time_Tracking/Attendance_Time_Tracking/wwwroot/ExcelFiles/Sheet.xlsx
+++ b/Attendance_Time_Tracking/Attendance_Time_Tracking/wwwroot/ExcelFiles/Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI-PD&amp;BI\MVC-Project\Project\Attendance-Time-tracking-System-\Attendance_Time_Tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30CF15E8-2CEC-4E03-9A42-9A1DB5E6CFB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891CA729-FBC1-441C-896C-BCD0FFC8A486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -411,7 +411,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,7 +483,7 @@
         <v>11</v>
       </c>
       <c r="J2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K2">
         <v>1</v>

</xml_diff>